<commit_message>
implement the export to excel of cajeros and selfs
</commit_message>
<xml_diff>
--- a/Plantilla_Exportada.xlsx
+++ b/Plantilla_Exportada.xlsx
@@ -3,26 +3,32 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,16 +49,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -60,7 +66,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -68,10 +74,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -80,23 +86,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -104,17 +110,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -122,7 +139,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -195,14 +212,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -229,116 +246,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,239 +333,263 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F1:F1048576"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11.42578125" customWidth="1" style="1" min="1" max="1"/>
-    <col width="43.7109375" customWidth="1" min="2" max="2"/>
-    <col width="11.42578125" customWidth="1" min="3" max="3"/>
-    <col width="8.7109375" customWidth="1" min="4" max="4"/>
-    <col width="43.7109375" customWidth="1" min="6" max="6"/>
-    <col width="8.7109375" customWidth="1" min="8" max="8"/>
+    <col width="11.43357142857143" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="43.71928571428572" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="11.43357142857143" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="8.719285714285713" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="43.71928571428572" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
+    <col width="8.719285714285713" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>UBICACIÓN DIARIA DE CAJEROS</t>
         </is>
       </c>
-      <c r="B1" s="5" t="n"/>
-      <c r="C1" s="5" t="n"/>
-      <c r="D1" s="5" t="n"/>
-      <c r="E1" s="5" t="n"/>
-      <c r="F1" s="5" t="n"/>
-      <c r="G1" s="5" t="n"/>
-      <c r="H1" s="6" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="B1" s="8" t="n"/>
+      <c r="C1" s="8" t="n"/>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="8" t="n"/>
+      <c r="F1" s="8" t="n"/>
+      <c r="G1" s="8" t="n"/>
+      <c r="H1" s="9" t="n"/>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>DOMINGO 20 DE OCTUBRE 2024</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n"/>
-      <c r="C2" s="5" t="n"/>
-      <c r="D2" s="5" t="n"/>
-      <c r="E2" s="5" t="n"/>
-      <c r="F2" s="5" t="n"/>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="6" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="B2" s="8" t="n"/>
+      <c r="C2" s="8" t="n"/>
+      <c r="D2" s="8" t="n"/>
+      <c r="E2" s="8" t="n"/>
+      <c r="F2" s="8" t="n"/>
+      <c r="G2" s="8" t="n"/>
+      <c r="H2" s="9" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Nº Caja</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>CAJERO(A) 1er Turno</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>TURNO</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>REFRIG</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>Nº Caja</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>CAJERO(A)</t>
         </is>
       </c>
-      <c r="G3" s="4" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>TURNO</t>
         </is>
       </c>
-      <c r="H3" s="4" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>REFRIG</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>1 PREF</t>
         </is>
@@ -598,7 +605,7 @@
         </is>
       </c>
       <c r="D4" s="3" t="n"/>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>1 PREF</t>
         </is>
@@ -615,8 +622,8 @@
       </c>
       <c r="H4" s="3" t="n"/>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="n"/>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="1" t="n"/>
       <c r="B5" s="3" t="inlineStr">
         <is>
           <t>(T) BRANCACHO RAMIREZ, BRINDY</t>
@@ -628,7 +635,7 @@
         </is>
       </c>
       <c r="D5" s="3" t="n"/>
-      <c r="E5" s="4" t="n"/>
+      <c r="E5" s="1" t="n"/>
       <c r="F5" s="3" t="inlineStr">
         <is>
           <t>(T) AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
@@ -641,8 +648,8 @@
       </c>
       <c r="H5" s="3" t="n"/>
     </row>
-    <row r="6">
-      <c r="A6" s="4" t="n">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -656,15 +663,15 @@
         </is>
       </c>
       <c r="D6" s="3" t="n"/>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="3" t="n"/>
       <c r="H6" s="3" t="n"/>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="n"/>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="1" t="n"/>
       <c r="B7" s="3" t="inlineStr">
         <is>
           <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
@@ -676,13 +683,13 @@
         </is>
       </c>
       <c r="D7" s="3" t="n"/>
-      <c r="E7" s="4" t="n"/>
+      <c r="E7" s="1" t="n"/>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="n">
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -696,49 +703,33 @@
         </is>
       </c>
       <c r="D8" s="3" t="n"/>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="inlineStr">
-        <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="inlineStr">
-        <is>
-          <t>15:45-19:15</t>
-        </is>
-      </c>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
       <c r="H8" s="3" t="n"/>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="n"/>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="1" t="n"/>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>DEL AGUILA MURAYARI, DARLA</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>12:00-15:45</t>
+          <t>12:00-21:00</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="inlineStr">
-        <is>
-          <t>19:15-22:00</t>
-        </is>
-      </c>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -752,15 +743,15 @@
         </is>
       </c>
       <c r="D10" s="3" t="n"/>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
       <c r="H10" s="3" t="n"/>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="n"/>
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="1" t="n"/>
       <c r="B11" s="3" t="inlineStr">
         <is>
           <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
@@ -772,13 +763,13 @@
         </is>
       </c>
       <c r="D11" s="3" t="n"/>
-      <c r="E11" s="4" t="n"/>
+      <c r="E11" s="1" t="n"/>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row r="12">
-      <c r="A12" s="4" t="n">
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -792,33 +783,41 @@
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>13:45-22:00</t>
+        </is>
+      </c>
       <c r="H12" s="3" t="n"/>
     </row>
-    <row r="13">
-      <c r="A13" s="4" t="n"/>
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="1" t="n"/>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:45</t>
+          <t>13:15-13:30</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
-      <c r="E13" s="4" t="n"/>
+      <c r="E13" s="1" t="n"/>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="n">
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -832,33 +831,33 @@
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="1" t="n">
         <v>6</v>
       </c>
       <c r="F14" s="3" t="n"/>
       <c r="G14" s="3" t="n"/>
       <c r="H14" s="3" t="n"/>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="n"/>
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="1" t="n"/>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
+          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>14:00-21:30</t>
+          <t>13:45-22:45</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
-      <c r="E15" s="4" t="n"/>
+      <c r="E15" s="1" t="n"/>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="n">
+    <row r="16" ht="18.75" customHeight="1">
+      <c r="A16" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -872,23 +871,23 @@
         </is>
       </c>
       <c r="D16" s="3" t="n"/>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="1" t="n">
         <v>7</v>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>14:15-22:45</t>
+          <t>14:00-21:30</t>
         </is>
       </c>
       <c r="H16" s="3" t="n"/>
     </row>
-    <row r="17">
-      <c r="A17" s="4" t="n"/>
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="A17" s="1" t="n"/>
       <c r="B17" s="3" t="inlineStr">
         <is>
           <t>CASAPAICO RIVERA, ENZO MANUEL</t>
@@ -900,13 +899,13 @@
         </is>
       </c>
       <c r="D17" s="3" t="n"/>
-      <c r="E17" s="4" t="n"/>
+      <c r="E17" s="1" t="n"/>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
       <c r="H17" s="3" t="n"/>
     </row>
-    <row r="18">
-      <c r="A18" s="4" t="n">
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -920,23 +919,23 @@
         </is>
       </c>
       <c r="D18" s="3" t="n"/>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="1" t="n">
         <v>8</v>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>19:00-22:45</t>
         </is>
       </c>
       <c r="H18" s="3" t="n"/>
     </row>
-    <row r="19">
-      <c r="A19" s="4" t="n"/>
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="1" t="n"/>
       <c r="B19" s="3" t="inlineStr">
         <is>
           <t>SICHA JORGE, JOSE ANGELO</t>
@@ -948,13 +947,13 @@
         </is>
       </c>
       <c r="D19" s="3" t="n"/>
-      <c r="E19" s="4" t="n"/>
+      <c r="E19" s="1" t="n"/>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
       <c r="H19" s="3" t="n"/>
     </row>
-    <row r="20">
-      <c r="A20" s="4" t="n">
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -968,33 +967,41 @@
         </is>
       </c>
       <c r="D20" s="3" t="n"/>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>19:15-22:00</t>
+        </is>
+      </c>
       <c r="H20" s="3" t="n"/>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="n"/>
+    <row r="21" ht="18.75" customHeight="1">
+      <c r="A21" s="1" t="n"/>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>16:00-19:45</t>
+          <t>15:45-19:15</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
-      <c r="E21" s="4" t="n"/>
+      <c r="E21" s="1" t="n"/>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
       <c r="H21" s="3" t="n"/>
     </row>
-    <row r="22">
-      <c r="A22" s="4" t="n">
+    <row r="22" ht="18.75" customHeight="1">
+      <c r="A22" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1008,33 +1015,33 @@
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
-      <c r="E22" s="4" t="n">
+      <c r="E22" s="1" t="n">
         <v>10</v>
       </c>
       <c r="F22" s="3" t="n"/>
       <c r="G22" s="3" t="n"/>
       <c r="H22" s="3" t="n"/>
     </row>
-    <row r="23">
-      <c r="A23" s="4" t="n"/>
+    <row r="23" ht="18.75" customHeight="1">
+      <c r="A23" s="1" t="n"/>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>16:45-20:30</t>
+          <t>16:00-19:45</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
-      <c r="E23" s="4" t="n"/>
+      <c r="E23" s="1" t="n"/>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
       <c r="H23" s="3" t="n"/>
     </row>
-    <row r="24">
-      <c r="A24" s="4" t="n">
+    <row r="24" ht="18.75" customHeight="1">
+      <c r="A24" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1048,102 +1055,102 @@
         </is>
       </c>
       <c r="D24" s="3" t="n"/>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="1" t="n">
         <v>11</v>
       </c>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
       <c r="H24" s="3" t="n"/>
     </row>
-    <row r="25">
-      <c r="A25" s="4" t="n"/>
+    <row r="25" ht="18.75" customHeight="1">
+      <c r="A25" s="1" t="n"/>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>16:45-20:30</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
-      <c r="E25" s="4" t="n"/>
+      <c r="E25" s="1" t="n"/>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
       <c r="H25" s="3" t="n"/>
     </row>
-    <row r="26">
-      <c r="A26" s="4" t="n">
+    <row r="26" ht="18.75" customHeight="1">
+      <c r="A26" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>DEL AGUILA MURAYARI, DARLA</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>14:15-22:45</t>
         </is>
       </c>
       <c r="D26" s="3" t="n"/>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="1" t="n">
         <v>12</v>
       </c>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="3" t="n"/>
     </row>
-    <row r="27">
-      <c r="A27" s="4" t="n"/>
+    <row r="27" ht="18.75" customHeight="1">
+      <c r="A27" s="1" t="n"/>
       <c r="B27" s="3" t="n"/>
       <c r="C27" s="3" t="n"/>
       <c r="D27" s="3" t="n"/>
-      <c r="E27" s="4" t="n"/>
+      <c r="E27" s="1" t="n"/>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
       <c r="H27" s="3" t="n"/>
     </row>
-    <row r="28">
-      <c r="A28" s="4" t="n">
+    <row r="28" ht="18.75" customHeight="1">
+      <c r="A28" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D28" s="3" t="n"/>
-      <c r="E28" s="4" t="n">
+      <c r="E28" s="1" t="n">
         <v>13</v>
       </c>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
       <c r="H28" s="3" t="n"/>
     </row>
-    <row r="29">
-      <c r="A29" s="4" t="n"/>
+    <row r="29" ht="18.75" customHeight="1">
+      <c r="A29" s="1" t="n"/>
       <c r="B29" s="3" t="n"/>
       <c r="C29" s="3" t="n"/>
       <c r="D29" s="3" t="n"/>
-      <c r="E29" s="4" t="n"/>
+      <c r="E29" s="1" t="n"/>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
       <c r="H29" s="3" t="n"/>
     </row>
-    <row r="30">
-      <c r="A30" s="4" t="n">
+    <row r="30" ht="18.75" customHeight="1">
+      <c r="A30" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1152,343 +1159,408 @@
         </is>
       </c>
       <c r="D30" s="3" t="n"/>
-      <c r="E30" s="4" t="n">
+      <c r="E30" s="1" t="n">
         <v>14</v>
       </c>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
     </row>
-    <row r="31">
-      <c r="A31" s="4" t="n"/>
+    <row r="31" ht="18.75" customHeight="1">
+      <c r="A31" s="1" t="n"/>
       <c r="B31" s="3" t="n"/>
       <c r="C31" s="3" t="n"/>
       <c r="D31" s="3" t="n"/>
-      <c r="E31" s="4" t="n"/>
+      <c r="E31" s="1" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
     </row>
-    <row r="32">
-      <c r="A32" s="4" t="n">
+    <row r="32" ht="18.75" customHeight="1">
+      <c r="A32" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>BRENIS LARTIGA, SEBASTIAN</t>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>18:00-21:45</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D32" s="3" t="n"/>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="1" t="n">
         <v>15</v>
       </c>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
     </row>
-    <row r="33">
-      <c r="A33" s="4" t="n"/>
+    <row r="33" ht="18.75" customHeight="1">
+      <c r="A33" s="1" t="n"/>
       <c r="B33" s="3" t="n"/>
       <c r="C33" s="3" t="n"/>
       <c r="D33" s="3" t="n"/>
-      <c r="E33" s="4" t="n"/>
+      <c r="E33" s="1" t="n"/>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
     </row>
-    <row r="34">
-      <c r="A34" s="4" t="n">
+    <row r="34" ht="18.75" customHeight="1">
+      <c r="A34" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B34" s="3" t="n"/>
       <c r="C34" s="3" t="n"/>
       <c r="D34" s="3" t="n"/>
-      <c r="E34" s="4" t="n">
+      <c r="E34" s="1" t="n">
         <v>16</v>
       </c>
       <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
     </row>
-    <row r="35">
-      <c r="A35" s="4" t="n"/>
+    <row r="35" ht="18.75" customHeight="1">
+      <c r="A35" s="1" t="n"/>
       <c r="B35" s="3" t="n"/>
       <c r="C35" s="3" t="n"/>
       <c r="D35" s="3" t="n"/>
-      <c r="E35" s="4" t="n"/>
+      <c r="E35" s="1" t="n"/>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
     </row>
-    <row r="36">
-      <c r="A36" s="4" t="n">
+    <row r="36" ht="18.75" customHeight="1">
+      <c r="A36" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B36" s="3" t="n"/>
       <c r="C36" s="3" t="n"/>
       <c r="D36" s="3" t="n"/>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="1" t="n">
         <v>17</v>
       </c>
       <c r="F36" s="3" t="n"/>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
     </row>
-    <row r="37">
-      <c r="A37" s="4" t="n"/>
+    <row r="37" ht="18.75" customHeight="1">
+      <c r="A37" s="1" t="n"/>
       <c r="B37" s="3" t="n"/>
       <c r="C37" s="3" t="n"/>
       <c r="D37" s="3" t="n"/>
-      <c r="E37" s="4" t="n"/>
+      <c r="E37" s="1" t="n"/>
       <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
     </row>
-    <row r="38">
-      <c r="A38" s="4" t="n">
+    <row r="38" ht="18.75" customHeight="1">
+      <c r="A38" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B38" s="3" t="n"/>
       <c r="C38" s="3" t="n"/>
       <c r="D38" s="3" t="n"/>
-      <c r="E38" s="4" t="n">
+      <c r="E38" s="1" t="n">
         <v>18</v>
       </c>
       <c r="F38" s="3" t="n"/>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
     </row>
-    <row r="39">
-      <c r="A39" s="4" t="n"/>
+    <row r="39" ht="18.75" customHeight="1">
+      <c r="A39" s="1" t="n"/>
       <c r="B39" s="3" t="n"/>
       <c r="C39" s="3" t="n"/>
       <c r="D39" s="3" t="n"/>
-      <c r="E39" s="3" t="n"/>
+      <c r="E39" s="4" t="n"/>
       <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
     </row>
-    <row r="40">
-      <c r="A40" s="4" t="inlineStr">
+    <row r="40" ht="18.75" customHeight="1">
+      <c r="A40" s="1" t="inlineStr">
         <is>
           <t>CAJA RAPIDA</t>
         </is>
       </c>
-      <c r="B40" s="5" t="n"/>
-      <c r="C40" s="5" t="n"/>
-      <c r="D40" s="5" t="n"/>
-      <c r="E40" s="5" t="n"/>
-      <c r="F40" s="5" t="n"/>
-      <c r="G40" s="5" t="n"/>
-      <c r="H40" s="6" t="n"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="B40" s="8" t="n"/>
+      <c r="C40" s="8" t="n"/>
+      <c r="D40" s="8" t="n"/>
+      <c r="E40" s="8" t="n"/>
+      <c r="F40" s="8" t="n"/>
+      <c r="G40" s="8" t="n"/>
+      <c r="H40" s="9" t="n"/>
+    </row>
+    <row r="41" ht="18.75" customHeight="1">
+      <c r="A41" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B41" s="3" t="n"/>
       <c r="C41" s="3" t="n"/>
       <c r="D41" s="3" t="n"/>
-      <c r="E41" s="4" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
       <c r="F41" s="3" t="n"/>
       <c r="G41" s="3" t="n"/>
       <c r="H41" s="3" t="n"/>
     </row>
-    <row r="42">
-      <c r="A42" s="4" t="n"/>
+    <row r="42" ht="18.75" customHeight="1">
+      <c r="A42" s="1" t="n"/>
       <c r="B42" s="3" t="n"/>
       <c r="C42" s="3" t="n"/>
       <c r="D42" s="3" t="n"/>
-      <c r="E42" s="4" t="n"/>
+      <c r="E42" s="1" t="n"/>
       <c r="F42" s="3" t="n"/>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
     </row>
-    <row r="43">
-      <c r="A43" s="4" t="n">
+    <row r="43" ht="18.75" customHeight="1">
+      <c r="A43" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>09:00-18:00</t>
+          <t>12:00-15:45</t>
         </is>
       </c>
       <c r="D43" s="3" t="n"/>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="1" t="n">
         <v>21</v>
       </c>
       <c r="F43" s="3" t="n"/>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
     </row>
-    <row r="44">
-      <c r="A44" s="4" t="n"/>
+    <row r="44" ht="18.75" customHeight="1">
+      <c r="A44" s="1" t="n"/>
       <c r="B44" s="3" t="n"/>
       <c r="C44" s="3" t="n"/>
       <c r="D44" s="3" t="n"/>
-      <c r="E44" s="4" t="n"/>
+      <c r="E44" s="1" t="n"/>
       <c r="F44" s="3" t="n"/>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
     </row>
-    <row r="45">
-      <c r="A45" s="4" t="n">
+    <row r="45" ht="18.75" customHeight="1">
+      <c r="A45" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>13:15-13:30</t>
+          <t>09:00-18:00</t>
         </is>
       </c>
       <c r="D45" s="3" t="n"/>
-      <c r="E45" s="4" t="n">
+      <c r="E45" s="1" t="n">
         <v>22</v>
       </c>
       <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
     </row>
-    <row r="46">
-      <c r="A46" s="4" t="n"/>
+    <row r="46" ht="18.75" customHeight="1">
+      <c r="A46" s="1" t="n"/>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:00</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
-      <c r="E46" s="4" t="n"/>
+      <c r="E46" s="1" t="n"/>
       <c r="F46" s="3" t="n"/>
       <c r="G46" s="3" t="n"/>
       <c r="H46" s="3" t="n"/>
     </row>
-    <row r="47">
-      <c r="A47" s="4" t="n">
+    <row r="47" ht="18.75" customHeight="1">
+      <c r="A47" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B47" s="3" t="n"/>
       <c r="C47" s="3" t="n"/>
       <c r="D47" s="3" t="n"/>
-      <c r="E47" s="4" t="n">
+      <c r="E47" s="1" t="n">
         <v>23</v>
       </c>
       <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
     </row>
-    <row r="48">
-      <c r="A48" s="4" t="n"/>
+    <row r="48" ht="18.75" customHeight="1">
+      <c r="A48" s="1" t="n"/>
       <c r="B48" s="3" t="n"/>
       <c r="C48" s="3" t="n"/>
       <c r="D48" s="3" t="n"/>
-      <c r="E48" s="4" t="n"/>
+      <c r="E48" s="1" t="n"/>
       <c r="F48" s="3" t="n"/>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
     </row>
-    <row r="49">
-      <c r="A49" s="4" t="n">
+    <row r="49" ht="18.75" customHeight="1">
+      <c r="A49" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B49" s="3" t="n"/>
       <c r="C49" s="3" t="n"/>
       <c r="D49" s="3" t="n"/>
-      <c r="E49" s="4" t="n">
+      <c r="E49" s="1" t="n">
         <v>24</v>
       </c>
       <c r="F49" s="3" t="n"/>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
     </row>
-    <row r="50">
-      <c r="A50" s="4" t="n"/>
+    <row r="50" ht="18.75" customHeight="1">
+      <c r="A50" s="1" t="n"/>
       <c r="B50" s="3" t="n"/>
       <c r="C50" s="3" t="n"/>
       <c r="D50" s="3" t="n"/>
-      <c r="E50" s="3" t="n"/>
+      <c r="E50" s="4" t="n"/>
       <c r="F50" s="3" t="n"/>
       <c r="G50" s="3" t="n"/>
       <c r="H50" s="3" t="n"/>
     </row>
-    <row r="51">
-      <c r="A51" s="4" t="inlineStr">
+    <row r="51" ht="18.75" customHeight="1">
+      <c r="A51" s="1" t="inlineStr">
         <is>
           <t>SELF CHECK OUT</t>
         </is>
       </c>
-      <c r="B51" s="5" t="n"/>
-      <c r="C51" s="5" t="n"/>
-      <c r="D51" s="5" t="n"/>
-      <c r="E51" s="5" t="n"/>
-      <c r="F51" s="5" t="n"/>
-      <c r="G51" s="5" t="n"/>
-      <c r="H51" s="6" t="n"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="inlineStr">
+      <c r="B51" s="8" t="n"/>
+      <c r="C51" s="8" t="n"/>
+      <c r="D51" s="8" t="n"/>
+      <c r="E51" s="8" t="n"/>
+      <c r="F51" s="8" t="n"/>
+      <c r="G51" s="8" t="n"/>
+      <c r="H51" s="9" t="n"/>
+    </row>
+    <row r="52" ht="18.75" customHeight="1">
+      <c r="A52" s="1" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="B52" s="3" t="n"/>
-      <c r="C52" s="3" t="n"/>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>HUAMANI QUICANO, EMELYN HEIDY</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>07:00-10:45</t>
+        </is>
+      </c>
       <c r="D52" s="3" t="n"/>
-      <c r="E52" s="4" t="inlineStr">
+      <c r="E52" s="1" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="F52" s="3" t="n"/>
-      <c r="G52" s="3" t="n"/>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>EVANGELISTA INFANTES, MARIA FERNANDA</t>
+        </is>
+      </c>
+      <c r="G52" s="3" t="inlineStr">
+        <is>
+          <t>15:15-19:00</t>
+        </is>
+      </c>
       <c r="H52" s="3" t="n"/>
     </row>
-    <row r="53">
-      <c r="A53" s="4" t="inlineStr">
+    <row r="53" ht="18.75" customHeight="1">
+      <c r="A53" s="1" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="B53" s="3" t="n"/>
-      <c r="C53" s="3" t="n"/>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>HUANUCO VICUÑA, ABIGAIL LUZ</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>10:45-14:30</t>
+        </is>
+      </c>
       <c r="D53" s="3" t="n"/>
-      <c r="E53" s="4" t="inlineStr">
+      <c r="E53" s="1" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="F53" s="3" t="n"/>
-      <c r="G53" s="3" t="n"/>
-      <c r="H53" s="3" t="n"/>
+      <c r="F53" s="7" t="inlineStr">
+        <is>
+          <t>ORIHUELA PUMACCAHUA, ALVARO RAUL</t>
+        </is>
+      </c>
+      <c r="G53" s="7" t="inlineStr">
+        <is>
+          <t>18:15-22:00</t>
+        </is>
+      </c>
+      <c r="H53" s="7" t="n"/>
+    </row>
+    <row r="54" ht="18.75" customHeight="1">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>25-30</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>CARHUANCHO RAYMUNDO, JAMES JESUS</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>14:30-18:15</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="n"/>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>25-30</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>MACHCO HUARCA, NICOLAS AXEL</t>
+        </is>
+      </c>
+      <c r="G54" s="3" t="inlineStr">
+        <is>
+          <t>19:00-22:45</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implement plantilla semanal (max 4 cajeros)
</commit_message>
<xml_diff>
--- a/Plantilla_Exportada.xlsx
+++ b/Plantilla_Exportada.xlsx
@@ -706,26 +706,42 @@
       <c r="E8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>15:45-19:15</t>
+        </is>
+      </c>
       <c r="H8" s="3" t="n"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>DEL AGUILA MURAYARI, DARLA</t>
+          <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>12:00-15:45</t>
         </is>
       </c>
       <c r="D9" s="3" t="n"/>
       <c r="E9" s="1" t="n"/>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>19:15-22:00</t>
+        </is>
+      </c>
       <c r="H9" s="3" t="n"/>
     </row>
     <row r="10" ht="18.75" customHeight="1">
@@ -786,28 +802,20 @@
       <c r="E12" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="inlineStr">
-        <is>
-          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>13:45-22:00</t>
-        </is>
-      </c>
+      <c r="F12" s="3" t="n"/>
+      <c r="G12" s="3" t="n"/>
       <c r="H12" s="3" t="n"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
+          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13:15-13:30</t>
+          <t>13:45-22:45</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
@@ -842,12 +850,12 @@
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
+          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:45</t>
+          <t>14:00-21:30</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
@@ -876,12 +884,12 @@
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
+          <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>14:00-21:30</t>
+          <t>14:15-22:45</t>
         </is>
       </c>
       <c r="H16" s="3" t="n"/>
@@ -924,12 +932,12 @@
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>ZAPATA VILLANUEVA, FIORELLA YASMIN</t>
+          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>19:00-22:45</t>
+          <t>18:15-22:00</t>
         </is>
       </c>
       <c r="H18" s="3" t="n"/>
@@ -970,28 +978,20 @@
       <c r="E20" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
-        <is>
-          <t>19:15-22:00</t>
-        </is>
-      </c>
+      <c r="F20" s="3" t="n"/>
+      <c r="G20" s="3" t="n"/>
       <c r="H20" s="3" t="n"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>ERIQUE CALLE, MARIA ANTONIETA</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>15:45-19:15</t>
+          <t>16:00-19:45</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
@@ -1026,12 +1026,12 @@
       <c r="A23" s="1" t="n"/>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>16:00-19:45</t>
+          <t>16:45-20:30</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
@@ -1066,12 +1066,12 @@
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>16:45-20:30</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>RAMOS TINOCO, JORDAN JAVIER</t>
+          <t>DEL AGUILA MURAYARI, DARLA</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>14:15-22:45</t>
+          <t>12:00-21:00</t>
         </is>
       </c>
       <c r="D26" s="3" t="n"/>
@@ -1118,12 +1118,12 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>17:30-21:15</t>
         </is>
       </c>
       <c r="D28" s="3" t="n"/>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1182,12 +1182,12 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
+          <t>BRENIS LARTIGA, SEBASTIAN</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>17:30-21:15</t>
+          <t>18:00-21:45</t>
         </is>
       </c>
       <c r="D32" s="3" t="n"/>
@@ -1324,12 +1324,12 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>YANQUI BRAVO, MIRIAN LUZ</t>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>12:00-15:45</t>
+          <t>09:00-18:00</t>
         </is>
       </c>
       <c r="D43" s="3" t="n"/>
@@ -1356,12 +1356,12 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>09:00-18:00</t>
+          <t>13:15-13:30</t>
         </is>
       </c>
       <c r="D45" s="3" t="n"/>
@@ -1376,12 +1376,12 @@
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
+          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>18:15-22:00</t>
+          <t>13:45-22:00</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>

</xml_diff>

<commit_message>
fixed script with new features, falta exportar pdf y registro de fijas para cajas rapidas
</commit_message>
<xml_diff>
--- a/Plantilla_Exportada.xlsx
+++ b/Plantilla_Exportada.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -27,7 +27,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -63,6 +63,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -110,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -121,20 +175,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,10 +294,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -257,71 +335,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -349,7 +427,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -372,11 +450,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -385,13 +463,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -401,7 +479,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -410,7 +488,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -419,7 +497,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -427,10 +505,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -498,1069 +576,1080 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="11.43357142857143" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="43.71928571428572" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
-    <col width="11.43357142857143" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
-    <col width="8.719285714285713" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
-    <col width="43.71928571428572" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
-    <col width="8.719285714285713" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="43.7109375" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
+    <col width="43.7109375" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>UBICACIÓN DIARIA DE CAJEROS</t>
         </is>
       </c>
-      <c r="B1" s="8" t="n"/>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="8" t="n"/>
-      <c r="G1" s="8" t="n"/>
-      <c r="H1" s="9" t="n"/>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="B1" s="16" t="n"/>
+      <c r="C1" s="16" t="n"/>
+      <c r="D1" s="16" t="n"/>
+      <c r="E1" s="16" t="n"/>
+      <c r="F1" s="16" t="n"/>
+      <c r="G1" s="16" t="n"/>
+      <c r="H1" s="17" t="n"/>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>DOMINGO 20 DE OCTUBRE 2024</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n"/>
-      <c r="C2" s="8" t="n"/>
-      <c r="D2" s="8" t="n"/>
-      <c r="E2" s="8" t="n"/>
-      <c r="F2" s="8" t="n"/>
-      <c r="G2" s="8" t="n"/>
-      <c r="H2" s="9" t="n"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="B2" s="16" t="n"/>
+      <c r="C2" s="16" t="n"/>
+      <c r="D2" s="16" t="n"/>
+      <c r="E2" s="16" t="n"/>
+      <c r="F2" s="16" t="n"/>
+      <c r="G2" s="16" t="n"/>
+      <c r="H2" s="17" t="n"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Nº Caja</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>CAJERO(A) 1er Turno</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="8" t="inlineStr">
         <is>
           <t>TURNO</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="8" t="inlineStr">
         <is>
           <t>REFRIG</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>Nº Caja</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="8" t="inlineStr">
         <is>
           <t>CAJERO(A)</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G3" s="8" t="inlineStr">
         <is>
           <t>TURNO</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="H3" s="8" t="inlineStr">
         <is>
           <t>REFRIG</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>1 PREF</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>HUAMAN HUAMANI, ALEXIS JAVIER</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="10" t="inlineStr">
         <is>
           <t>06:30-10:15</t>
         </is>
       </c>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="1" t="inlineStr">
+      <c r="D4" s="10" t="n"/>
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>1 PREF</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="10" t="inlineStr">
+        <is>
+          <t>(T) AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
+        </is>
+      </c>
+      <c r="G4" s="10" t="inlineStr">
+        <is>
+          <t>22:00-22:45</t>
+        </is>
+      </c>
+      <c r="H4" s="10" t="n"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="13" t="n"/>
+      <c r="B5" s="14" t="inlineStr">
+        <is>
+          <t>(T) BRANCACHO RAMIREZ, BRINDY</t>
+        </is>
+      </c>
+      <c r="C5" s="14" t="inlineStr">
+        <is>
+          <t>10:00-13:45</t>
+        </is>
+      </c>
+      <c r="D5" s="14" t="n"/>
+      <c r="E5" s="13" t="n"/>
+      <c r="F5" s="14" t="n"/>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="14" t="n"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="11" t="n"/>
+      <c r="B6" s="12" t="inlineStr">
         <is>
           <t>(T) JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
+      <c r="C6" s="12" t="inlineStr">
         <is>
           <t>13:30-22:15</t>
         </is>
       </c>
-      <c r="H4" s="3" t="n"/>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>(T) BRANCACHO RAMIREZ, BRINDY</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>10:00-13:45</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="1" t="n"/>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>(T) AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="inlineStr">
-        <is>
-          <t>22:00-22:45</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="n"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="1" t="n">
+      <c r="D6" s="12" t="n"/>
+      <c r="E6" s="11" t="n"/>
+      <c r="F6" s="12" t="n"/>
+      <c r="G6" s="12" t="n"/>
+      <c r="H6" s="12" t="n"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>LOPEZ SANCHEZ, NELLY ANDREA</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>07:00-16:00</t>
         </is>
       </c>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="1" t="n">
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
-    </row>
-    <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>16:00-19:45</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="1" t="n"/>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
     </row>
-    <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="1" t="n">
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>LIZARME HUINCHO, BRIYITH JASUMI</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>16:00-19:45</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="3" t="n"/>
+    </row>
+    <row r="9" ht="19.5" customHeight="1">
+      <c r="A9" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>QUISPE MONDRAGON, JUAN ALFONSO</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>08:15-12:00</t>
         </is>
       </c>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" s="1" t="n">
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>ERIQUE CALLE, MARIA ANTONIETA</t>
         </is>
       </c>
-      <c r="G8" s="3" t="inlineStr">
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t>15:45-19:15</t>
         </is>
       </c>
-      <c r="H8" s="3" t="n"/>
-    </row>
-    <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="H9" s="3" t="n"/>
+    </row>
+    <row r="10" ht="19.5" customHeight="1">
+      <c r="A10" s="7" t="n"/>
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>YANQUI BRAVO, MIRIAN LUZ</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>12:00-15:45</t>
         </is>
       </c>
-      <c r="D9" s="3" t="n"/>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="3" t="inlineStr">
         <is>
           <t>VILCAPOMA CHILIN, JULISSA JAZMIN</t>
         </is>
       </c>
-      <c r="G9" s="3" t="inlineStr">
+      <c r="G10" s="3" t="inlineStr">
         <is>
           <t>19:15-22:00</t>
         </is>
       </c>
-      <c r="H9" s="3" t="n"/>
-    </row>
-    <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="1" t="n">
+      <c r="H10" s="3" t="n"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1">
+      <c r="A11" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>VEGA CARDENAS, ANGELICA LOURDES</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>08:45-12:30</t>
         </is>
       </c>
-      <c r="D10" s="3" t="n"/>
-      <c r="E10" s="1" t="n">
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
-      <c r="H10" s="3" t="n"/>
-    </row>
-    <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="1" t="n"/>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>12:45-21:45</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="1" t="n"/>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
     </row>
-    <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="1" t="n">
-        <v>5</v>
-      </c>
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="A12" s="7" t="n"/>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>ROA ZARATE, ELIZABETH LUCY</t>
+          <t>QUISPE MENDOZA, ANTONY MAURICIO</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>09:30-13:15</t>
+          <t>12:45-21:45</t>
         </is>
       </c>
       <c r="D12" s="3" t="n"/>
-      <c r="E12" s="1" t="n">
-        <v>5</v>
-      </c>
+      <c r="E12" s="7" t="n"/>
       <c r="F12" s="3" t="n"/>
       <c r="G12" s="3" t="n"/>
       <c r="H12" s="3" t="n"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="1" t="n"/>
+    <row r="13" ht="19.5" customHeight="1">
+      <c r="A13" s="7" t="n">
+        <v>5</v>
+      </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
+          <t>ROA ZARATE, ELIZABETH LUCY</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:45</t>
+          <t>09:30-13:15</t>
         </is>
       </c>
       <c r="D13" s="3" t="n"/>
-      <c r="E13" s="1" t="n"/>
+      <c r="E13" s="7" t="n">
+        <v>5</v>
+      </c>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
     </row>
-    <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="1" t="n">
-        <v>6</v>
-      </c>
+    <row r="14" ht="19.5" customHeight="1">
+      <c r="A14" s="7" t="n"/>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>HUAYANAY VELASCO, ATHINA</t>
+          <t>HEREDIA CAHUAYA, SUSAN NAYELLI</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>10:00-13:45</t>
+          <t>13:45-22:45</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
-      <c r="E14" s="1" t="n">
-        <v>6</v>
-      </c>
+      <c r="E14" s="7" t="n"/>
       <c r="F14" s="3" t="n"/>
       <c r="G14" s="3" t="n"/>
       <c r="H14" s="3" t="n"/>
     </row>
-    <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="1" t="n"/>
+    <row r="15" ht="19.5" customHeight="1">
+      <c r="A15" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
+          <t>HUAYANAY VELASCO, ATHINA</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>14:00-21:30</t>
+          <t>10:00-13:45</t>
         </is>
       </c>
       <c r="D15" s="3" t="n"/>
-      <c r="E15" s="1" t="n"/>
+      <c r="E15" s="7" t="n">
+        <v>6</v>
+      </c>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="1" t="n">
+    <row r="16" ht="19.5" customHeight="1">
+      <c r="A16" s="7" t="n"/>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>HURTADO SAMPLINI, JACK FERNANDO</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>14:00-21:30</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n"/>
+      <c r="E16" s="7" t="n"/>
+      <c r="F16" s="3" t="n"/>
+      <c r="G16" s="3" t="n"/>
+      <c r="H16" s="3" t="n"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1">
+      <c r="A17" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>BRANCACHO RAMIREZ, BRINDY</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>10:00-10:00</t>
         </is>
       </c>
-      <c r="D16" s="3" t="n"/>
-      <c r="E16" s="1" t="n">
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="F16" s="3" t="inlineStr">
+      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>RAMOS TINOCO, JORDAN JAVIER</t>
         </is>
       </c>
-      <c r="G16" s="3" t="inlineStr">
+      <c r="G17" s="3" t="inlineStr">
         <is>
           <t>14:15-22:45</t>
         </is>
       </c>
-      <c r="H16" s="3" t="n"/>
-    </row>
-    <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="1" t="n"/>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="H17" s="3" t="n"/>
+    </row>
+    <row r="18" ht="19.5" customHeight="1">
+      <c r="A18" s="7" t="n"/>
+      <c r="B18" s="3" t="inlineStr">
         <is>
           <t>CASAPAICO RIVERA, ENZO MANUEL</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>10:15-14:00</t>
         </is>
       </c>
-      <c r="D17" s="3" t="n"/>
-      <c r="E17" s="1" t="n"/>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
-      <c r="H17" s="3" t="n"/>
-    </row>
-    <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="1" t="n">
+      <c r="D18" s="3" t="n"/>
+      <c r="E18" s="7" t="n"/>
+      <c r="F18" s="3" t="n"/>
+      <c r="G18" s="3" t="n"/>
+      <c r="H18" s="3" t="n"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1">
+      <c r="A19" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>SOTO VELAZCO, EMIR ALESSANDRO</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>10:45-14:30</t>
         </is>
       </c>
-      <c r="D18" s="3" t="n"/>
-      <c r="E18" s="1" t="n">
+      <c r="D19" s="3" t="n"/>
+      <c r="E19" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="F18" s="3" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>LA ROSA EUSEBIO, SHADIA SHAMIRA</t>
         </is>
       </c>
-      <c r="G18" s="3" t="inlineStr">
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>18:15-22:00</t>
         </is>
       </c>
-      <c r="H18" s="3" t="n"/>
-    </row>
-    <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="1" t="n"/>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="H19" s="3" t="n"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="3" t="inlineStr">
         <is>
           <t>SICHA JORGE, JOSE ANGELO</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
+      <c r="C20" s="3" t="inlineStr">
         <is>
           <t>14:30-18:15</t>
         </is>
       </c>
-      <c r="D19" s="3" t="n"/>
-      <c r="E19" s="1" t="n"/>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
-      <c r="H19" s="3" t="n"/>
-    </row>
-    <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B20" s="3" t="inlineStr">
-        <is>
-          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
-        </is>
-      </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>10:45-14:30</t>
-        </is>
-      </c>
       <c r="D20" s="3" t="n"/>
-      <c r="E20" s="1" t="n">
-        <v>9</v>
-      </c>
+      <c r="E20" s="7" t="n"/>
       <c r="F20" s="3" t="n"/>
       <c r="G20" s="3" t="n"/>
       <c r="H20" s="3" t="n"/>
     </row>
-    <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="1" t="n"/>
+    <row r="21" ht="19.5" customHeight="1">
+      <c r="A21" s="7" t="n">
+        <v>9</v>
+      </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>PEREZ GORMAS, ANTHONY</t>
+          <t>RUIZ SANTOS, CIELO CRISTHINA</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>16:00-19:45</t>
+          <t>10:45-14:30</t>
         </is>
       </c>
       <c r="D21" s="3" t="n"/>
-      <c r="E21" s="1" t="n"/>
+      <c r="E21" s="7" t="n">
+        <v>9</v>
+      </c>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
       <c r="H21" s="3" t="n"/>
     </row>
-    <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="1" t="n">
-        <v>10</v>
-      </c>
+    <row r="22" ht="19.5" customHeight="1">
+      <c r="A22" s="7" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
+          <t>PEREZ GORMAS, ANTHONY</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>11:00-14:45</t>
+          <t>16:00-19:45</t>
         </is>
       </c>
       <c r="D22" s="3" t="n"/>
-      <c r="E22" s="1" t="n">
-        <v>10</v>
-      </c>
+      <c r="E22" s="7" t="n"/>
       <c r="F22" s="3" t="n"/>
       <c r="G22" s="3" t="n"/>
       <c r="H22" s="3" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="1" t="n"/>
+    <row r="23" ht="19.5" customHeight="1">
+      <c r="A23" s="7" t="n">
+        <v>10</v>
+      </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
+          <t>CUSI QUISPE, ANDREA ESTEFANY</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>16:45-20:30</t>
+          <t>11:00-14:45</t>
         </is>
       </c>
       <c r="D23" s="3" t="n"/>
-      <c r="E23" s="1" t="n"/>
+      <c r="E23" s="7" t="n">
+        <v>10</v>
+      </c>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
       <c r="H23" s="3" t="n"/>
     </row>
     <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="A24" s="7" t="n"/>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
+          <t>GARRIDO SOTO, VICTORIA CELESTE</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>11:15-15:00</t>
+          <t>16:45-20:30</t>
         </is>
       </c>
       <c r="D24" s="3" t="n"/>
-      <c r="E24" s="1" t="n">
-        <v>11</v>
-      </c>
+      <c r="E24" s="7" t="n"/>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
       <c r="H24" s="3" t="n"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
-      <c r="A25" s="1" t="n"/>
+      <c r="A25" s="7" t="n">
+        <v>11</v>
+      </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>LEON TICONA, MARIA FERNANDA</t>
+          <t>QUIQUIA MALLQUI, CYNTHIA ANGELLINE</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>17:00-20:45</t>
+          <t>11:15-15:00</t>
         </is>
       </c>
       <c r="D25" s="3" t="n"/>
-      <c r="E25" s="1" t="n"/>
+      <c r="E25" s="7" t="n">
+        <v>11</v>
+      </c>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
       <c r="H25" s="3" t="n"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
-      <c r="A26" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="A26" s="7" t="n"/>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>DEL AGUILA MURAYARI, DARLA</t>
+          <t>LEON TICONA, MARIA FERNANDA</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>12:00-21:00</t>
+          <t>17:00-20:45</t>
         </is>
       </c>
       <c r="D26" s="3" t="n"/>
-      <c r="E26" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="E26" s="7" t="n"/>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="3" t="n"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="1" t="n"/>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="3" t="n"/>
+      <c r="A27" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>DEL AGUILA MURAYARI, DARLA</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>12:00-21:00</t>
+        </is>
+      </c>
       <c r="D27" s="3" t="n"/>
-      <c r="E27" s="1" t="n"/>
+      <c r="E27" s="7" t="n">
+        <v>12</v>
+      </c>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
       <c r="H27" s="3" t="n"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B28" s="3" t="inlineStr">
-        <is>
-          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
-        </is>
-      </c>
-      <c r="C28" s="3" t="inlineStr">
-        <is>
-          <t>17:30-21:15</t>
-        </is>
-      </c>
+      <c r="A28" s="7" t="n"/>
+      <c r="B28" s="3" t="n"/>
+      <c r="C28" s="3" t="n"/>
       <c r="D28" s="3" t="n"/>
-      <c r="E28" s="1" t="n">
-        <v>13</v>
-      </c>
+      <c r="E28" s="7" t="n"/>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
       <c r="H28" s="3" t="n"/>
     </row>
     <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="1" t="n"/>
-      <c r="B29" s="3" t="n"/>
-      <c r="C29" s="3" t="n"/>
+      <c r="A29" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>IDELFONSO MOTTA, JHOSSEP ANGELO</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>17:30-21:15</t>
+        </is>
+      </c>
       <c r="D29" s="3" t="n"/>
-      <c r="E29" s="1" t="n"/>
+      <c r="E29" s="7" t="n">
+        <v>13</v>
+      </c>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
       <c r="H29" s="3" t="n"/>
     </row>
     <row r="30" ht="18.75" customHeight="1">
-      <c r="A30" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3" t="inlineStr">
-        <is>
-          <t>INGA DELGADO, CARLOS DANIEL</t>
-        </is>
-      </c>
-      <c r="C30" s="3" t="inlineStr">
-        <is>
-          <t>17:30-21:15</t>
-        </is>
-      </c>
+      <c r="A30" s="7" t="n"/>
+      <c r="B30" s="3" t="n"/>
+      <c r="C30" s="3" t="n"/>
       <c r="D30" s="3" t="n"/>
-      <c r="E30" s="1" t="n">
-        <v>14</v>
-      </c>
+      <c r="E30" s="7" t="n"/>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
     </row>
     <row r="31" ht="18.75" customHeight="1">
-      <c r="A31" s="1" t="n"/>
-      <c r="B31" s="3" t="n"/>
-      <c r="C31" s="3" t="n"/>
+      <c r="A31" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>INGA DELGADO, CARLOS DANIEL</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>17:30-21:15</t>
+        </is>
+      </c>
       <c r="D31" s="3" t="n"/>
-      <c r="E31" s="1" t="n"/>
+      <c r="E31" s="7" t="n">
+        <v>14</v>
+      </c>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
     </row>
     <row r="32" ht="18.75" customHeight="1">
-      <c r="A32" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B32" s="3" t="inlineStr">
-        <is>
-          <t>BRENIS LARTIGA, SEBASTIAN</t>
-        </is>
-      </c>
-      <c r="C32" s="3" t="inlineStr">
-        <is>
-          <t>18:00-21:45</t>
-        </is>
-      </c>
+      <c r="A32" s="7" t="n"/>
+      <c r="B32" s="3" t="n"/>
+      <c r="C32" s="3" t="n"/>
       <c r="D32" s="3" t="n"/>
-      <c r="E32" s="1" t="n">
-        <v>15</v>
-      </c>
+      <c r="E32" s="7" t="n"/>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
-      <c r="A33" s="1" t="n"/>
-      <c r="B33" s="3" t="n"/>
-      <c r="C33" s="3" t="n"/>
+      <c r="A33" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>BRENIS LARTIGA, SEBASTIAN</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>18:00-21:45</t>
+        </is>
+      </c>
       <c r="D33" s="3" t="n"/>
-      <c r="E33" s="1" t="n"/>
+      <c r="E33" s="7" t="n">
+        <v>15</v>
+      </c>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
     </row>
     <row r="34" ht="18.75" customHeight="1">
-      <c r="A34" s="1" t="n">
-        <v>16</v>
-      </c>
+      <c r="A34" s="7" t="n"/>
       <c r="B34" s="3" t="n"/>
       <c r="C34" s="3" t="n"/>
       <c r="D34" s="3" t="n"/>
-      <c r="E34" s="1" t="n">
-        <v>16</v>
-      </c>
+      <c r="E34" s="7" t="n"/>
       <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
     </row>
     <row r="35" ht="18.75" customHeight="1">
-      <c r="A35" s="1" t="n"/>
+      <c r="A35" s="7" t="n">
+        <v>16</v>
+      </c>
       <c r="B35" s="3" t="n"/>
       <c r="C35" s="3" t="n"/>
       <c r="D35" s="3" t="n"/>
-      <c r="E35" s="1" t="n"/>
+      <c r="E35" s="7" t="n">
+        <v>16</v>
+      </c>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
     </row>
     <row r="36" ht="18.75" customHeight="1">
-      <c r="A36" s="1" t="n">
-        <v>17</v>
-      </c>
+      <c r="A36" s="7" t="n"/>
       <c r="B36" s="3" t="n"/>
       <c r="C36" s="3" t="n"/>
       <c r="D36" s="3" t="n"/>
-      <c r="E36" s="1" t="n">
-        <v>17</v>
-      </c>
+      <c r="E36" s="7" t="n"/>
       <c r="F36" s="3" t="n"/>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
     </row>
     <row r="37" ht="18.75" customHeight="1">
-      <c r="A37" s="1" t="n"/>
+      <c r="A37" s="7" t="n">
+        <v>17</v>
+      </c>
       <c r="B37" s="3" t="n"/>
       <c r="C37" s="3" t="n"/>
       <c r="D37" s="3" t="n"/>
-      <c r="E37" s="1" t="n"/>
+      <c r="E37" s="7" t="n">
+        <v>17</v>
+      </c>
       <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
     </row>
     <row r="38" ht="18.75" customHeight="1">
-      <c r="A38" s="1" t="n">
-        <v>18</v>
-      </c>
+      <c r="A38" s="7" t="n"/>
       <c r="B38" s="3" t="n"/>
       <c r="C38" s="3" t="n"/>
       <c r="D38" s="3" t="n"/>
-      <c r="E38" s="1" t="n">
-        <v>18</v>
-      </c>
+      <c r="E38" s="7" t="n"/>
       <c r="F38" s="3" t="n"/>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
     </row>
     <row r="39" ht="18.75" customHeight="1">
-      <c r="A39" s="1" t="n"/>
+      <c r="A39" s="7" t="n">
+        <v>18</v>
+      </c>
       <c r="B39" s="3" t="n"/>
       <c r="C39" s="3" t="n"/>
       <c r="D39" s="3" t="n"/>
-      <c r="E39" s="4" t="n"/>
+      <c r="E39" s="7" t="n">
+        <v>18</v>
+      </c>
       <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
     </row>
     <row r="40" ht="18.75" customHeight="1">
-      <c r="A40" s="1" t="inlineStr">
+      <c r="A40" s="7" t="n"/>
+      <c r="B40" s="3" t="n"/>
+      <c r="C40" s="3" t="n"/>
+      <c r="D40" s="3" t="n"/>
+      <c r="E40" s="6" t="n"/>
+      <c r="F40" s="3" t="n"/>
+      <c r="G40" s="3" t="n"/>
+      <c r="H40" s="3" t="n"/>
+    </row>
+    <row r="41" ht="18.75" customHeight="1">
+      <c r="A41" s="7" t="inlineStr">
         <is>
           <t>CAJA RAPIDA</t>
         </is>
       </c>
-      <c r="B40" s="8" t="n"/>
-      <c r="C40" s="8" t="n"/>
-      <c r="D40" s="8" t="n"/>
-      <c r="E40" s="8" t="n"/>
-      <c r="F40" s="8" t="n"/>
-      <c r="G40" s="8" t="n"/>
-      <c r="H40" s="9" t="n"/>
-    </row>
-    <row r="41" ht="18.75" customHeight="1">
-      <c r="A41" s="1" t="n">
+      <c r="B41" s="16" t="n"/>
+      <c r="C41" s="16" t="n"/>
+      <c r="D41" s="16" t="n"/>
+      <c r="E41" s="16" t="n"/>
+      <c r="F41" s="16" t="n"/>
+      <c r="G41" s="16" t="n"/>
+      <c r="H41" s="17" t="n"/>
+    </row>
+    <row r="42" ht="18.75" customHeight="1">
+      <c r="A42" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="B41" s="3" t="n"/>
-      <c r="C41" s="3" t="n"/>
-      <c r="D41" s="3" t="n"/>
-      <c r="E41" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F41" s="3" t="n"/>
-      <c r="G41" s="3" t="n"/>
-      <c r="H41" s="3" t="n"/>
-    </row>
-    <row r="42" ht="18.75" customHeight="1">
-      <c r="A42" s="1" t="n"/>
       <c r="B42" s="3" t="n"/>
       <c r="C42" s="3" t="n"/>
       <c r="D42" s="3" t="n"/>
-      <c r="E42" s="1" t="n"/>
+      <c r="E42" s="7" t="n">
+        <v>20</v>
+      </c>
       <c r="F42" s="3" t="n"/>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
     </row>
     <row r="43" ht="18.75" customHeight="1">
-      <c r="A43" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B43" s="3" t="inlineStr">
-        <is>
-          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
-        </is>
-      </c>
-      <c r="C43" s="3" t="inlineStr">
-        <is>
-          <t>09:00-18:00</t>
-        </is>
-      </c>
+      <c r="A43" s="7" t="n"/>
+      <c r="B43" s="3" t="n"/>
+      <c r="C43" s="3" t="n"/>
       <c r="D43" s="3" t="n"/>
-      <c r="E43" s="1" t="n">
-        <v>21</v>
-      </c>
+      <c r="E43" s="7" t="n"/>
       <c r="F43" s="3" t="n"/>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
     </row>
     <row r="44" ht="18.75" customHeight="1">
-      <c r="A44" s="1" t="n"/>
-      <c r="B44" s="3" t="n"/>
-      <c r="C44" s="3" t="n"/>
+      <c r="A44" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>MARTINEZ PAZ, ROCIO ESPERANZA</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>09:00-18:00</t>
+        </is>
+      </c>
       <c r="D44" s="3" t="n"/>
-      <c r="E44" s="1" t="n"/>
+      <c r="E44" s="7" t="n">
+        <v>21</v>
+      </c>
       <c r="F44" s="3" t="n"/>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
-      <c r="A45" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
-        </is>
-      </c>
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>13:15-13:30</t>
-        </is>
-      </c>
+      <c r="A45" s="7" t="n"/>
+      <c r="B45" s="3" t="n"/>
+      <c r="C45" s="3" t="n"/>
       <c r="D45" s="3" t="n"/>
-      <c r="E45" s="1" t="n">
-        <v>22</v>
-      </c>
+      <c r="E45" s="7" t="n"/>
       <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
     </row>
     <row r="46" ht="18.75" customHeight="1">
-      <c r="A46" s="1" t="n"/>
+      <c r="A46" s="7" t="n">
+        <v>22</v>
+      </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
+          <t>JIMENEZ TORERO, ASTRID GERALDINE</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>13:45-22:00</t>
+          <t>13:15-13:30</t>
         </is>
       </c>
       <c r="D46" s="3" t="n"/>
-      <c r="E46" s="1" t="n"/>
+      <c r="E46" s="7" t="n">
+        <v>22</v>
+      </c>
       <c r="F46" s="3" t="n"/>
       <c r="G46" s="3" t="n"/>
       <c r="H46" s="3" t="n"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
-      <c r="A47" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B47" s="3" t="n"/>
-      <c r="C47" s="3" t="n"/>
+      <c r="A47" s="7" t="n"/>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>AYQUIPA MONTENEGRO, VALERIA ESTEFANY</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="inlineStr">
+        <is>
+          <t>13:45-22:00</t>
+        </is>
+      </c>
       <c r="D47" s="3" t="n"/>
-      <c r="E47" s="1" t="n">
-        <v>23</v>
-      </c>
+      <c r="E47" s="7" t="n"/>
       <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
-      <c r="A48" s="1" t="n"/>
+      <c r="A48" s="7" t="n">
+        <v>23</v>
+      </c>
       <c r="B48" s="3" t="n"/>
       <c r="C48" s="3" t="n"/>
       <c r="D48" s="3" t="n"/>
-      <c r="E48" s="1" t="n"/>
+      <c r="E48" s="7" t="n">
+        <v>23</v>
+      </c>
       <c r="F48" s="3" t="n"/>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
     </row>
     <row r="49" ht="18.75" customHeight="1">
-      <c r="A49" s="1" t="n">
-        <v>24</v>
-      </c>
+      <c r="A49" s="7" t="n"/>
       <c r="B49" s="3" t="n"/>
       <c r="C49" s="3" t="n"/>
       <c r="D49" s="3" t="n"/>
-      <c r="E49" s="1" t="n">
-        <v>24</v>
-      </c>
+      <c r="E49" s="7" t="n"/>
       <c r="F49" s="3" t="n"/>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
     </row>
     <row r="50" ht="18.75" customHeight="1">
-      <c r="A50" s="1" t="n"/>
+      <c r="A50" s="7" t="n">
+        <v>24</v>
+      </c>
       <c r="B50" s="3" t="n"/>
       <c r="C50" s="3" t="n"/>
       <c r="D50" s="3" t="n"/>
-      <c r="E50" s="4" t="n"/>
+      <c r="E50" s="7" t="n">
+        <v>24</v>
+      </c>
       <c r="F50" s="3" t="n"/>
       <c r="G50" s="3" t="n"/>
       <c r="H50" s="3" t="n"/>
     </row>
     <row r="51" ht="18.75" customHeight="1">
-      <c r="A51" s="1" t="inlineStr">
+      <c r="A51" s="7" t="n"/>
+      <c r="B51" s="3" t="n"/>
+      <c r="C51" s="3" t="n"/>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="6" t="n"/>
+      <c r="F51" s="3" t="n"/>
+      <c r="G51" s="3" t="n"/>
+      <c r="H51" s="3" t="n"/>
+    </row>
+    <row r="52" ht="18.75" customHeight="1">
+      <c r="A52" s="7" t="inlineStr">
         <is>
           <t>SELF CHECK OUT</t>
         </is>
       </c>
-      <c r="B51" s="8" t="n"/>
-      <c r="C51" s="8" t="n"/>
-      <c r="D51" s="8" t="n"/>
-      <c r="E51" s="8" t="n"/>
-      <c r="F51" s="8" t="n"/>
-      <c r="G51" s="8" t="n"/>
-      <c r="H51" s="9" t="n"/>
-    </row>
-    <row r="52" ht="18.75" customHeight="1">
-      <c r="A52" s="1" t="inlineStr">
+      <c r="B52" s="16" t="n"/>
+      <c r="C52" s="16" t="n"/>
+      <c r="D52" s="16" t="n"/>
+      <c r="E52" s="16" t="n"/>
+      <c r="F52" s="16" t="n"/>
+      <c r="G52" s="16" t="n"/>
+      <c r="H52" s="17" t="n"/>
+    </row>
+    <row r="53" ht="18.75" customHeight="1">
+      <c r="A53" s="7" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="B52" s="3" t="inlineStr">
+      <c r="B53" s="3" t="inlineStr">
         <is>
           <t>HUAMANI QUICANO, EMELYN HEIDY</t>
         </is>
       </c>
-      <c r="C52" s="3" t="inlineStr">
+      <c r="C53" s="3" t="inlineStr">
         <is>
           <t>07:00-10:45</t>
         </is>
       </c>
-      <c r="D52" s="3" t="n"/>
-      <c r="E52" s="1" t="inlineStr">
+      <c r="D53" s="3" t="n"/>
+      <c r="E53" s="7" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="F52" s="3" t="inlineStr">
+      <c r="F53" s="10" t="inlineStr">
         <is>
           <t>EVANGELISTA INFANTES, MARIA FERNANDA</t>
         </is>
       </c>
-      <c r="G52" s="3" t="inlineStr">
+      <c r="G53" s="10" t="inlineStr">
         <is>
           <t>15:15-19:00</t>
         </is>
       </c>
-      <c r="H52" s="3" t="n"/>
-    </row>
-    <row r="53" ht="18.75" customHeight="1">
-      <c r="A53" s="1" t="inlineStr">
+      <c r="H53" s="10" t="n"/>
+    </row>
+    <row r="54" ht="18.75" customHeight="1">
+      <c r="A54" s="7" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="B53" s="3" t="inlineStr">
+      <c r="B54" s="3" t="inlineStr">
         <is>
           <t>HUANUCO VICUÑA, ABIGAIL LUZ</t>
         </is>
       </c>
-      <c r="C53" s="3" t="inlineStr">
+      <c r="C54" s="3" t="inlineStr">
         <is>
           <t>10:45-14:30</t>
         </is>
       </c>
-      <c r="D53" s="3" t="n"/>
-      <c r="E53" s="1" t="inlineStr">
+      <c r="D54" s="3" t="n"/>
+      <c r="E54" s="15" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="F53" s="7" t="inlineStr">
+      <c r="F54" s="14" t="inlineStr">
         <is>
           <t>ORIHUELA PUMACCAHUA, ALVARO RAUL</t>
         </is>
       </c>
-      <c r="G53" s="7" t="inlineStr">
+      <c r="G54" s="14" t="inlineStr">
         <is>
           <t>18:15-22:00</t>
         </is>
       </c>
-      <c r="H53" s="7" t="n"/>
-    </row>
-    <row r="54" ht="18.75" customHeight="1">
-      <c r="A54" s="1" t="inlineStr">
+      <c r="H54" s="14" t="n"/>
+    </row>
+    <row r="55" ht="18.75" customHeight="1">
+      <c r="A55" s="7" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="B54" s="3" t="inlineStr">
+      <c r="B55" s="3" t="inlineStr">
         <is>
           <t>CARHUANCHO RAYMUNDO, JAMES JESUS</t>
         </is>
       </c>
-      <c r="C54" s="3" t="inlineStr">
+      <c r="C55" s="3" t="inlineStr">
         <is>
           <t>14:30-18:15</t>
         </is>
       </c>
-      <c r="D54" s="3" t="n"/>
-      <c r="E54" s="1" t="inlineStr">
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="7" t="inlineStr">
         <is>
           <t>25-30</t>
         </is>
       </c>
-      <c r="F54" s="3" t="inlineStr">
+      <c r="F55" s="12" t="inlineStr">
         <is>
           <t>MACHCO HUARCA, NICOLAS AXEL</t>
         </is>
       </c>
-      <c r="G54" s="3" t="inlineStr">
+      <c r="G55" s="12" t="inlineStr">
         <is>
           <t>19:00-22:45</t>
         </is>
       </c>
-      <c r="H54" s="3" t="n"/>
+      <c r="H55" s="12" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A52:H52"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A40:H40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="56"/>
 </worksheet>
 </file>
</xml_diff>